<commit_message>
New metadata from @wilsonsj100 and reworked steps
</commit_message>
<xml_diff>
--- a/test/COMPASS_ChamberFlux_Metadata_2022_06_Gcrew.xlsx
+++ b/test/COMPASS_ChamberFlux_Metadata_2022_06_Gcrew.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Biogeochemistry\People\Wilson (Steph)\Data\Fluxes\Chamber Fluxes\June 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Biogeochemistry\People\Wilson (Steph)\Data\Fluxes\Chamber Fluxes\Data for Ben\June_2022_GCrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2187CEC-63CA-43D2-931B-04BEBC273711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624143E1-61AE-4BCC-9D4E-9AD8300E3FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{43107FA4-7C6A-8A41-9858-E4BE7819DE13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43107FA4-7C6A-8A41-9858-E4BE7819DE13}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPASS_ChamberFlux_Metadata_20" sheetId="1" r:id="rId1"/>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used redo </t>
   </si>
 </sst>
 </file>
@@ -710,12 +713,13 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A2:XFD15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" style="2"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -761,7 +765,7 @@
         <v>44722</v>
       </c>
       <c r="B2" s="2">
-        <v>0.56770833333333337</v>
+        <v>0.57500000000000007</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -792,7 +796,7 @@
         <v>24.444400000000002</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>